<commit_message>
backup for pc switch
</commit_message>
<xml_diff>
--- a/aa.xlsx
+++ b/aa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\source\repos\TROLlox78\parseEquationValue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1760DA-3674-4CB2-BFBE-C589C8B38741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891CE3B5-538D-40CE-9D21-2E5CE953DBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="0" windowWidth="12075" windowHeight="16200" xr2:uid="{8721A5AD-F8B0-4928-A1B0-A8C767E4C737}"/>
+    <workbookView xWindow="885" yWindow="1485" windowWidth="12090" windowHeight="13965" xr2:uid="{8721A5AD-F8B0-4928-A1B0-A8C767E4C737}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="137">
   <si>
     <t>A</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>rpi1[Ω]</t>
-  </si>
-  <si>
-    <t>11 813,20</t>
   </si>
   <si>
     <t>re1[Ω]</t>
@@ -7295,8 +7292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986EC5E9-E0C8-4C3F-9331-94AADD43A3C1}">
   <dimension ref="A5:AI71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z45" sqref="Z45"/>
+    <sheetView tabSelected="1" topLeftCell="Z34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF45" sqref="AF45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8694,7 +8691,7 @@
       <c r="Y32" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="Z32" s="24">
+      <c r="Z32" s="25">
         <f>((I44+I45)*I34)/(I43+I44+I45)</f>
         <v>5.2467532467532472</v>
       </c>
@@ -8878,8 +8875,8 @@
       <c r="AB35" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AC35" s="12" t="s">
-        <v>109</v>
+      <c r="AC35" s="12">
+        <v>11813.2</v>
       </c>
       <c r="AE35" s="32" t="s">
         <v>66</v>
@@ -8934,7 +8931,7 @@
         <v>8.292971734148205</v>
       </c>
       <c r="AB36" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AC36" s="12">
         <v>49.017429450000002</v>
@@ -8989,7 +8986,7 @@
         <v>2.5207792207792208</v>
       </c>
       <c r="AB37" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AC37" s="12">
         <v>4075.9290059999998</v>
@@ -9027,7 +9024,7 @@
         <v>4.546753246753247</v>
       </c>
       <c r="AB38" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AC38" s="12">
         <v>3.29</v>
@@ -9065,7 +9062,7 @@
         <v>2.0259740259740262</v>
       </c>
       <c r="AB39" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AC39" s="11">
         <v>5.0799999999999999E-4</v>
@@ -9106,7 +9103,7 @@
         <v>3.746218487394958</v>
       </c>
       <c r="AB40" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC40" s="12">
         <v>5.6</v>
@@ -9146,7 +9143,7 @@
         <v>1.977081741787624E-2</v>
       </c>
       <c r="AB41" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AC41" s="12">
         <v>0.02</v>
@@ -9184,7 +9181,7 @@
         <v>1.977081741787624E-2</v>
       </c>
       <c r="AB42" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC42" s="12">
         <v>11813.200500000001</v>
@@ -9222,7 +9219,7 @@
         <v>12139.103554868625</v>
       </c>
       <c r="AB43" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC43" s="12">
         <v>49.017429450000002</v>
@@ -9231,7 +9228,7 @@
         <v>74</v>
       </c>
       <c r="AF43" s="24">
-        <f t="shared" ref="AF43" si="13">$I$31/AF41</f>
+        <f>I31/AF41</f>
         <v>11813.200498132008</v>
       </c>
       <c r="AG43" s="9"/>
@@ -9260,7 +9257,7 @@
         <v>12139.103554868625</v>
       </c>
       <c r="AB44" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AC44" s="12">
         <v>48.55</v>
@@ -9269,7 +9266,7 @@
         <v>75</v>
       </c>
       <c r="AF44" s="24">
-        <f t="shared" ref="AF44" si="14">$I$31/AF42</f>
+        <f>I31/AF42</f>
         <v>11813.200498132008</v>
       </c>
       <c r="AG44" s="9"/>
@@ -9417,7 +9414,7 @@
         <v>1.6488128893711507E-11</v>
       </c>
       <c r="AB48" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC48" s="12">
         <v>0.89073257049999999</v>
@@ -9464,7 +9461,7 @@
         <v>1999.6841103061538</v>
       </c>
       <c r="AB49" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC49" s="12">
         <v>0.49524011810000002</v>
@@ -9511,7 +9508,7 @@
         <v>7500</v>
       </c>
       <c r="AB50" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC50" s="12">
         <v>151.2376342</v>
@@ -9593,7 +9590,7 @@
         <v>-117.24958096787151</v>
       </c>
       <c r="AB52" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC52" s="12">
         <v>478.33</v>
@@ -9610,7 +9607,7 @@
     </row>
     <row r="53" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R53" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S53" s="27">
         <f>SQRT(S48*S52)</f>
@@ -9690,7 +9687,7 @@
         <v>9.0187500000000005E-12</v>
       </c>
       <c r="AB56" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC56" s="11">
         <v>7.8500000000000008E-9</v>
@@ -9731,7 +9728,7 @@
     </row>
     <row r="58" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K58" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L58" s="42" t="s">
         <v>9</v>
@@ -9773,7 +9770,7 @@
     </row>
     <row r="59" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C59" s="42" t="s">
         <v>0</v>
@@ -9787,31 +9784,31 @@
       <c r="H59" s="43"/>
       <c r="K59" s="9"/>
       <c r="L59" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="M59" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="M59" s="50" t="s">
-        <v>126</v>
-      </c>
       <c r="N59" s="64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O59" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="P59" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="P59" s="58" t="s">
-        <v>126</v>
-      </c>
       <c r="Q59" s="64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R59" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="S59" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="S59" s="58" t="s">
-        <v>126</v>
-      </c>
       <c r="T59" s="64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y59" s="32" t="s">
         <v>88</v>
@@ -9845,71 +9842,71 @@
     <row r="60" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="9"/>
       <c r="C60" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="D60" s="50" t="s">
-        <v>126</v>
-      </c>
       <c r="E60" s="64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F60" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="G60" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="G60" s="50" t="s">
-        <v>126</v>
-      </c>
       <c r="H60" s="64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K60" s="48" t="s">
         <v>104</v>
       </c>
       <c r="L60" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M60" s="15">
         <f>Z31</f>
         <v>3.220779220779221</v>
       </c>
       <c r="N60" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O60" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P60" s="15">
         <f>AC31</f>
         <v>3.2902999999999998</v>
       </c>
       <c r="Q60" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R60" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S60" s="15">
         <f>AF31</f>
         <v>3.290322580645161</v>
       </c>
       <c r="T60" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y60" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z60" s="24">
         <f>1/(2*3.14*SQRT((Z57*Z57)+(Z58*Z58)+(Z59*Z59)))</f>
         <v>871707.64931984048</v>
       </c>
       <c r="AB60" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC60" s="12">
         <v>23840.33</v>
       </c>
       <c r="AE60" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AF60" s="25">
         <f>1/(2*3.14*SQRT((AF57*AF57)+(AF58*AF58)+(AF59*AF59)+(AH59*AH59)))</f>
@@ -9923,55 +9920,55 @@
         <v>18</v>
       </c>
       <c r="C61" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D61" s="44">
         <v>3.290322580645161</v>
       </c>
       <c r="E61" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F61" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G61" s="14">
         <v>3.290322580645161</v>
       </c>
       <c r="H61" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K61" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L61" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M61" s="15">
         <f>Z32</f>
         <v>5.2467532467532472</v>
       </c>
       <c r="N61" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O61" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P61" s="15">
         <f>AC38</f>
         <v>3.29</v>
       </c>
       <c r="Q61" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R61" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S61" s="15">
         <f>AF32</f>
         <v>3.290322580645161</v>
       </c>
       <c r="T61" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y61" s="32" t="s">
         <v>90</v>
@@ -10001,56 +9998,56 @@
         <v>19</v>
       </c>
       <c r="C62" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D62" s="44">
         <f>S32*1000</f>
         <v>507.90638836179625</v>
       </c>
       <c r="E62" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F62" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G62" s="15">
         <v>507.90638836179625</v>
       </c>
       <c r="H62" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K62" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L62" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M62" s="15">
         <f>Z33*1000</f>
         <v>0.49427043544690608</v>
       </c>
       <c r="N62" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O62" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P62" s="15">
         <f>AC32*1000</f>
         <v>0.50800000000000001</v>
       </c>
       <c r="Q62" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R62" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S62" s="15">
         <f>AF33*1000</f>
         <v>0.50790638836179625</v>
       </c>
       <c r="T62" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y62" s="32" t="s">
         <v>91</v>
@@ -10080,55 +10077,55 @@
         <v>20</v>
       </c>
       <c r="C63" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D63" s="44">
         <v>5.6003999999999996</v>
       </c>
       <c r="E63" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F63" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G63" s="15">
         <v>5.6003999999999996</v>
       </c>
       <c r="H63" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K63" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L63" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M63" s="15">
         <f>Z34*1000</f>
         <v>0.49427043544690608</v>
       </c>
       <c r="N63" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O63" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P63" s="15">
         <f>AC39*1000</f>
         <v>0.50800000000000001</v>
       </c>
       <c r="Q63" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R63" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S63" s="15">
         <f>AF34*1000</f>
         <v>0.50790638836179625</v>
       </c>
       <c r="T63" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y63" s="32" t="s">
         <v>92</v>
@@ -10149,7 +10146,7 @@
     </row>
     <row r="64" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C64" s="53">
         <f>L31/1000</f>
@@ -10160,7 +10157,7 @@
         <v>3.4811009174311924</v>
       </c>
       <c r="E64" s="65">
-        <f t="shared" ref="E64:E69" si="15">ABS((C64-D64)/((C64+D64)/2)*100)</f>
+        <f t="shared" ref="E64:E69" si="13">ABS((C64-D64)/((C64+D64)/2)*100)</f>
         <v>0.81188562944025522</v>
       </c>
       <c r="F64" s="53">
@@ -10172,41 +10169,41 @@
         <v>4.8550795104998906E-2</v>
       </c>
       <c r="H64" s="65">
-        <f t="shared" ref="H64:H69" si="16">ABS((F64-G64)/((F64+G64)/2)*100)</f>
+        <f t="shared" ref="H64:H69" si="14">ABS((F64-G64)/((F64+G64)/2)*100)</f>
         <v>8.0661950870168493</v>
       </c>
       <c r="K64" s="48" t="s">
         <v>106</v>
       </c>
       <c r="L64" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M64" s="15">
         <f>Z39</f>
         <v>2.0259740259740262</v>
       </c>
       <c r="N64" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O64" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P64" s="15">
         <f>AC33</f>
         <v>9.41</v>
       </c>
       <c r="Q64" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R64" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S64" s="15">
         <f>AF39</f>
         <v>9.4096774193548391</v>
       </c>
       <c r="T64" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y64" s="32" t="s">
         <v>93</v>
@@ -10216,7 +10213,7 @@
         <v>4192.4090627585474</v>
       </c>
       <c r="AB64" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AC64" s="34">
         <f>SQRT(AC63*AC57)</f>
@@ -10234,59 +10231,59 @@
     </row>
     <row r="65" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C65" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D65" s="45">
         <f>S39/1000</f>
         <v>7.5</v>
       </c>
       <c r="E65" s="66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F65" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G65" s="15">
         <v>7.5</v>
       </c>
       <c r="H65" s="66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K65" s="48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L65" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M65" s="15">
         <f>Z40</f>
         <v>3.746218487394958</v>
       </c>
       <c r="N65" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O65" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P65" s="15">
         <f>AC40</f>
         <v>5.6</v>
       </c>
       <c r="Q65" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R65" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S65" s="15">
         <f>AF40</f>
         <v>5.6003795066413682</v>
       </c>
       <c r="T65" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y65" s="32" t="s">
         <v>94</v>
@@ -10324,7 +10321,7 @@
         <v>-132.24318555663604</v>
       </c>
       <c r="E66" s="65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>5.7913891321550182</v>
       </c>
       <c r="F66" s="51">
@@ -10335,11 +10332,11 @@
         <v>13.385647160189091</v>
       </c>
       <c r="H66" s="65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>2.15699588884089</v>
       </c>
       <c r="K66" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L66" s="53">
         <f>N31/1000</f>
@@ -10403,7 +10400,7 @@
     </row>
     <row r="67" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C67" s="53">
         <f>B33</f>
@@ -10414,7 +10411,7 @@
         <v>3.9999149102664688</v>
       </c>
       <c r="E67" s="65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>11.766825786209045</v>
       </c>
       <c r="F67" s="53">
@@ -10426,40 +10423,40 @@
         <v>2.9028431802130528</v>
       </c>
       <c r="H67" s="65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>3.2918651849883815</v>
       </c>
       <c r="K67" s="48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L67" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M67" s="15">
         <f>Z50/1000</f>
         <v>7.5</v>
       </c>
       <c r="N67" s="66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O67" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P67" s="15">
         <f>AC45/1000</f>
         <v>7.5</v>
       </c>
       <c r="Q67" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R67" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S67" s="15">
         <v>7.5</v>
       </c>
       <c r="T67" s="66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y67" s="32" t="s">
         <v>96</v>
@@ -10487,7 +10484,7 @@
     </row>
     <row r="68" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C68" s="53">
         <f>B35</f>
@@ -10498,7 +10495,7 @@
         <v>445.81168739477738</v>
       </c>
       <c r="E68" s="65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>21.298198757133971</v>
       </c>
       <c r="F68" s="53">
@@ -10510,7 +10507,7 @@
         <v>873.08060223704945</v>
       </c>
       <c r="H68" s="65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>5.0591383849316047</v>
       </c>
       <c r="K68" s="48" t="s">
@@ -10525,7 +10522,7 @@
         <v>-117.24958096787151</v>
       </c>
       <c r="N68" s="65">
-        <f t="shared" ref="N68:N71" si="17">ABS((L68-M68)/((L68+M68)/2)*100)</f>
+        <f t="shared" ref="N68:N71" si="15">ABS((L68-M68)/((L68+M68)/2)*100)</f>
         <v>13.910704778136985</v>
       </c>
       <c r="O68" s="51">
@@ -10537,7 +10534,7 @@
         <v>66.714928760000006</v>
       </c>
       <c r="Q68" s="54">
-        <f t="shared" ref="Q68:Q71" si="18">ABS((O68-P68)/((O68+P68)/2)*100)</f>
+        <f t="shared" ref="Q68:Q71" si="16">ABS((O68-P68)/((O68+P68)/2)*100)</f>
         <v>13.975758710925323</v>
       </c>
       <c r="R68" s="51">
@@ -10549,7 +10546,7 @@
         <v>134.02809812484497</v>
       </c>
       <c r="T68" s="65">
-        <f t="shared" ref="T68:T71" si="19">ABS((R68-S68)/((R68+S68)/2)*100)</f>
+        <f t="shared" ref="T68:T71" si="17">ABS((R68-S68)/((R68+S68)/2)*100)</f>
         <v>10.21699037920698</v>
       </c>
       <c r="Y68" s="32" t="s">
@@ -10572,7 +10569,7 @@
     </row>
     <row r="69" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C69" s="62">
         <f>B34</f>
@@ -10583,7 +10580,7 @@
         <v>42.228057208228556</v>
       </c>
       <c r="E69" s="67">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>4.7965659599246999</v>
       </c>
       <c r="F69" s="55">
@@ -10595,11 +10592,11 @@
         <v>50.342984337245284</v>
       </c>
       <c r="H69" s="67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0.68362395141156829</v>
       </c>
       <c r="K69" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L69" s="53">
         <f>D33</f>
@@ -10610,7 +10607,7 @@
         <v>6.3703067483950244</v>
       </c>
       <c r="N69" s="65">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>16.289376610011828</v>
       </c>
       <c r="O69" s="53">
@@ -10622,7 +10619,7 @@
         <v>16.5</v>
       </c>
       <c r="Q69" s="54">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>16.393442622950818</v>
       </c>
       <c r="R69" s="53">
@@ -10634,7 +10631,7 @@
         <v>2.989636012979735</v>
       </c>
       <c r="T69" s="65">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>12.844674913771692</v>
       </c>
       <c r="Y69" s="32" t="s">
@@ -10656,7 +10653,7 @@
     </row>
     <row r="70" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K70" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L70" s="53">
         <f>D35</f>
@@ -10667,7 +10664,7 @@
         <v>871.70764931984047</v>
       </c>
       <c r="N70" s="65">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>4.901858358162837</v>
       </c>
       <c r="O70" s="53">
@@ -10679,7 +10676,7 @@
         <v>872</v>
       </c>
       <c r="Q70" s="54">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.7383177570093453</v>
       </c>
       <c r="R70" s="53">
@@ -10691,18 +10688,18 @@
         <v>871.45288223871569</v>
       </c>
       <c r="T70" s="65">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>6.08386822701386</v>
       </c>
       <c r="Y70" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Z70" s="28">
         <f>SQRT(Z60*Z69)</f>
         <v>74518.756840742746</v>
       </c>
       <c r="AE70" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AF70" s="28">
         <f>SQRT(AF69*AF60)</f>
@@ -10714,7 +10711,7 @@
     </row>
     <row r="71" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K71" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L71" s="55">
         <f>D34</f>
@@ -10725,7 +10722,7 @@
         <v>74.518756840742739</v>
       </c>
       <c r="N71" s="67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>5.8380399261648686</v>
       </c>
       <c r="O71" s="55">
@@ -10737,7 +10734,7 @@
         <v>119.9499895789908</v>
       </c>
       <c r="Q71" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>10.484746764903715</v>
       </c>
       <c r="R71" s="55">
@@ -10749,7 +10746,7 @@
         <v>51.042403160077136</v>
       </c>
       <c r="T71" s="67">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>3.3851235842711707</v>
       </c>
     </row>

</xml_diff>